<commit_message>
entorno y control de alistamiento
</commit_message>
<xml_diff>
--- a/Files/Temp_alist_adm/900258456_3/900258456_3.xlsx
+++ b/Files/Temp_alist_adm/900258456_3/900258456_3.xlsx
@@ -4,21 +4,36 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="20115" windowHeight="7485"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="T_OPERADORES">Hoja2!$A$1:$B$6</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>Guia N°</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="47">
+  <si>
+    <t>Guia</t>
+  </si>
+  <si>
+    <t>No venta</t>
+  </si>
+  <si>
+    <t>SKU</t>
+  </si>
+  <si>
+    <t>Cantidad</t>
+  </si>
+  <si>
+    <t>Operador</t>
   </si>
   <si>
     <t>Nombre Destinatario</t>
@@ -27,38 +42,131 @@
     <t>Direccion Destinatario</t>
   </si>
   <si>
-    <t>Ciudad Destino</t>
-  </si>
-  <si>
-    <t>Departamento Destino</t>
-  </si>
-  <si>
-    <t>Telefono Destino</t>
-  </si>
-  <si>
-    <t>Empresa Destino</t>
-  </si>
-  <si>
-    <t>Producto</t>
-  </si>
-  <si>
-    <t>Direccion Remite</t>
-  </si>
-  <si>
-    <t>Ciudad Remite</t>
-  </si>
-  <si>
-    <t>Referencia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identificacion </t>
+    <t>FMAP0006</t>
+  </si>
+  <si>
+    <t>XDAP0003</t>
+  </si>
+  <si>
+    <t>XMAP0006</t>
+  </si>
+  <si>
+    <t>FUAP0001</t>
+  </si>
+  <si>
+    <t>IGSG0011</t>
+  </si>
+  <si>
+    <t>FUSG0041</t>
+  </si>
+  <si>
+    <t>FUSG0044</t>
+  </si>
+  <si>
+    <t>XDSG0025</t>
+  </si>
+  <si>
+    <t>DWSG0003</t>
+  </si>
+  <si>
+    <t>FUSG0042</t>
+  </si>
+  <si>
+    <t>FUSG0045</t>
+  </si>
+  <si>
+    <t>FUSG0043</t>
+  </si>
+  <si>
+    <t>FUSG0046</t>
+  </si>
+  <si>
+    <t>FUSG0049</t>
+  </si>
+  <si>
+    <t>FUSG0050</t>
+  </si>
+  <si>
+    <t>XDSG0029</t>
+  </si>
+  <si>
+    <t>SLSG0043</t>
+  </si>
+  <si>
+    <t>FSSG0064</t>
+  </si>
+  <si>
+    <t>FUSG0031</t>
+  </si>
+  <si>
+    <t>FUSG0008</t>
+  </si>
+  <si>
+    <t>FUSG0014</t>
+  </si>
+  <si>
+    <t>XDSG0001</t>
+  </si>
+  <si>
+    <t>DEPRISA</t>
+  </si>
+  <si>
+    <t>Cod. OP</t>
+  </si>
+  <si>
+    <t>SERVIENTREGA</t>
+  </si>
+  <si>
+    <t>FEDEX</t>
+  </si>
+  <si>
+    <t>FUSG0025</t>
+  </si>
+  <si>
+    <t>FUSG0026</t>
+  </si>
+  <si>
+    <t>XDSG0018</t>
+  </si>
+  <si>
+    <t>ESSG0013</t>
+  </si>
+  <si>
+    <t>ESSG0007</t>
+  </si>
+  <si>
+    <t>FXHW0019</t>
+  </si>
+  <si>
+    <t>FXHW0020</t>
+  </si>
+  <si>
+    <t>XDHW0004</t>
+  </si>
+  <si>
+    <t>FXHW0013</t>
+  </si>
+  <si>
+    <t>FXHW0014</t>
+  </si>
+  <si>
+    <t>FXHW0016</t>
+  </si>
+  <si>
+    <t>LOGI YA FLEX</t>
+  </si>
+  <si>
+    <t>OPERADORES</t>
+  </si>
+  <si>
+    <t>INTERAPIDISIMO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,10 +176,18 @@
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF660066"/>
-      <name val="Eras Medium ITC"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -83,18 +199,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FF9FC5E8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF99FF66"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -103,45 +219,97 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFA9A9A9"/>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
       </left>
-      <right style="thin">
-        <color rgb="FFA9A9A9"/>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
       </right>
-      <top style="thin">
-        <color rgb="FFA9A9A9"/>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFA9A9A9"/>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <mruColors>
-      <color rgb="FF99FF66"/>
-      <color rgb="FF00FF99"/>
-      <color rgb="FF99FFCC"/>
-    </mruColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -437,33 +605,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H2" sqref="H2:H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -475,41 +638,876 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2005325410</v>
+      </c>
+      <c r="B2">
+        <v>302158965</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2">
+        <f>VLOOKUP(E2,T_OPERADORES,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2005325411</v>
+      </c>
+      <c r="B3" s="3">
+        <v>302158966</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="5">
+        <f>VLOOKUP(E3,T_OPERADORES,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>2005325412</v>
+      </c>
+      <c r="B4" s="3">
+        <v>302158967</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="5">
+        <f>VLOOKUP(E4,T_OPERADORES,2,FALSE)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>2005325413</v>
+      </c>
+      <c r="B5" s="3">
+        <v>302158968</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="5">
+        <f>VLOOKUP(E5,T_OPERADORES,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>2005325413</v>
+      </c>
+      <c r="B6" s="5">
+        <v>302158968</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="5">
+        <f>VLOOKUP(E6,T_OPERADORES,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
+        <v>2005325413</v>
+      </c>
+      <c r="B7" s="5">
+        <v>302158968</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="5">
+        <f>VLOOKUP(E7,T_OPERADORES,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>2005325416</v>
+      </c>
+      <c r="B8" s="3">
+        <v>302158971</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="5">
+        <f>VLOOKUP(E8,T_OPERADORES,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>2005325417</v>
+      </c>
+      <c r="B9" s="3">
+        <v>302158972</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="5">
+        <f>VLOOKUP(E9,T_OPERADORES,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>2005325418</v>
+      </c>
+      <c r="B10" s="3">
+        <v>302158973</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="5">
+        <f>VLOOKUP(E10,T_OPERADORES,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>2005325419</v>
+      </c>
+      <c r="B11" s="3">
+        <v>302158974</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H11" s="5">
+        <f>VLOOKUP(E11,T_OPERADORES,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>2005325420</v>
+      </c>
+      <c r="B12" s="3">
+        <v>302158975</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="5">
+        <f>VLOOKUP(E12,T_OPERADORES,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>2005325421</v>
+      </c>
+      <c r="B13" s="3">
+        <v>302158976</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="5">
+        <f>VLOOKUP(E13,T_OPERADORES,2,FALSE)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>2005325422</v>
+      </c>
+      <c r="B14" s="3">
+        <v>302158977</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" s="5">
+        <f>VLOOKUP(E14,T_OPERADORES,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>2005325423</v>
+      </c>
+      <c r="B15" s="3">
+        <v>302158978</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>29</v>
+      </c>
+      <c r="H15" s="5">
+        <f>VLOOKUP(E15,T_OPERADORES,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>2005325423</v>
+      </c>
+      <c r="B16" s="3">
+        <v>302158978</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" s="5">
+        <f>VLOOKUP(E16,T_OPERADORES,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>2005325425</v>
+      </c>
+      <c r="B17" s="3">
+        <v>302158980</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="5">
+        <f>VLOOKUP(E17,T_OPERADORES,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>2005325426</v>
+      </c>
+      <c r="B18" s="3">
+        <v>302158981</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" s="5">
+        <f>VLOOKUP(E18,T_OPERADORES,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>2005325427</v>
+      </c>
+      <c r="B19" s="3">
+        <v>302158982</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" s="5">
+        <f>VLOOKUP(E19,T_OPERADORES,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>2005325428</v>
+      </c>
+      <c r="B20" s="3">
+        <v>302158983</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" s="5">
+        <f>VLOOKUP(E20,T_OPERADORES,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>2005325429</v>
+      </c>
+      <c r="B21" s="3">
+        <v>302158984</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>31</v>
+      </c>
+      <c r="H21" s="5">
+        <f>VLOOKUP(E21,T_OPERADORES,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>2005325429</v>
+      </c>
+      <c r="B22" s="3">
+        <v>302158984</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>31</v>
+      </c>
+      <c r="H22" s="5">
+        <f>VLOOKUP(E22,T_OPERADORES,2,FALSE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>2005325431</v>
+      </c>
+      <c r="B23" s="3">
+        <v>302158986</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>29</v>
+      </c>
+      <c r="H23" s="5">
+        <f>VLOOKUP(E23,T_OPERADORES,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>2005325432</v>
+      </c>
+      <c r="B24" s="3">
+        <v>302158987</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H24" s="5">
+        <f>VLOOKUP(E24,T_OPERADORES,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>2005325433</v>
+      </c>
+      <c r="B25" s="3">
+        <v>302158988</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H25" s="5">
+        <f>VLOOKUP(E25,T_OPERADORES,2,FALSE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="5">
+        <v>2005325434</v>
+      </c>
+      <c r="B26" s="5">
+        <v>302158989</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>44</v>
+      </c>
+      <c r="H26" s="5">
+        <f>VLOOKUP(E26,T_OPERADORES,2,FALSE)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="5">
+        <v>2005325435</v>
+      </c>
+      <c r="B27" s="5">
+        <v>302158990</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H27" s="5">
+        <f>VLOOKUP(E27,T_OPERADORES,2,FALSE)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="5">
+        <v>2005325436</v>
+      </c>
+      <c r="B28" s="5">
+        <v>302158991</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H28" s="5">
+        <f>VLOOKUP(E28,T_OPERADORES,2,FALSE)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="5">
+        <v>2005325437</v>
+      </c>
+      <c r="B29" s="5">
+        <v>302158992</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H29" s="5">
+        <f>VLOOKUP(E29,T_OPERADORES,2,FALSE)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="5">
+        <v>2005325438</v>
+      </c>
+      <c r="B30" s="5">
+        <v>302158993</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H30" s="5">
+        <f>VLOOKUP(E30,T_OPERADORES,2,FALSE)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="5">
+        <v>2005325439</v>
+      </c>
+      <c r="B31" s="5">
+        <v>302158994</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H31" s="5">
+        <f>VLOOKUP(E31,T_OPERADORES,2,FALSE)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="5">
+        <v>2005325440</v>
+      </c>
+      <c r="B32" s="5">
+        <v>302158995</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H32" s="5">
+        <f>VLOOKUP(E32,T_OPERADORES,2,FALSE)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="5">
+        <v>2005325441</v>
+      </c>
+      <c r="B33" s="5">
+        <v>302158996</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33">
+        <v>3</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H33" s="5">
+        <f>VLOOKUP(E33,T_OPERADORES,2,FALSE)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="5">
+        <v>2005325442</v>
+      </c>
+      <c r="B34" s="5">
+        <v>302158997</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H34" s="5">
+        <f>VLOOKUP(E34,T_OPERADORES,2,FALSE)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="5">
+        <v>2005325443</v>
+      </c>
+      <c r="B35" s="5">
+        <v>302158998</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H35" s="5">
+        <f>VLOOKUP(E35,T_OPERADORES,2,FALSE)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="5">
+        <v>2005325444</v>
+      </c>
+      <c r="B36" s="5">
+        <v>302158999</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H36" s="5">
+        <f>VLOOKUP(E36,T_OPERADORES,2,FALSE)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="5">
+        <v>2005325445</v>
+      </c>
+      <c r="B37" s="5">
+        <v>302159000</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H37" s="5">
+        <f>VLOOKUP(E37,T_OPERADORES,2,FALSE)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="5">
+        <v>2005325446</v>
+      </c>
+      <c r="B38" s="5">
+        <v>302159001</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="H38" s="5">
+        <f>VLOOKUP(E38,T_OPERADORES,2,FALSE)</f>
+        <v>4</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C3">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C38">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B38">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="7"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>